<commit_message>
Te lo pedimos señor :,v
</commit_message>
<xml_diff>
--- a/digitales.xlsx
+++ b/digitales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\POO\Salvemos_POO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Salvemos_POO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{4A35DF11-C0D3-4648-94AC-2DEBBFF6F172}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{88C03B15-C237-4250-B53E-0A78EF24C246}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A9FFFF-D698-4677-BB7B-8C993D75F5F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{315B49EF-762D-468C-9D03-9D82A768DD0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{315B49EF-762D-468C-9D03-9D82A768DD0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Album1</t>
   </si>
@@ -41,18 +41,6 @@
     <t>Album3</t>
   </si>
   <si>
-    <t>Cancion 1</t>
-  </si>
-  <si>
-    <t>Cancion 2</t>
-  </si>
-  <si>
-    <t>Cancion 3</t>
-  </si>
-  <si>
-    <t>genero3</t>
-  </si>
-  <si>
     <t>path1</t>
   </si>
   <si>
@@ -62,16 +50,124 @@
     <t>path3</t>
   </si>
   <si>
-    <t>cantante1</t>
-  </si>
-  <si>
-    <t>cantante2</t>
-  </si>
-  <si>
-    <t>cantante3</t>
-  </si>
-  <si>
-    <t>cumbia</t>
+    <t>path4</t>
+  </si>
+  <si>
+    <t>path5</t>
+  </si>
+  <si>
+    <t>path6</t>
+  </si>
+  <si>
+    <t>path7</t>
+  </si>
+  <si>
+    <t>path8</t>
+  </si>
+  <si>
+    <t>path9</t>
+  </si>
+  <si>
+    <t>path10</t>
+  </si>
+  <si>
+    <t>chata</t>
+  </si>
+  <si>
+    <t>Cumbion</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Nacional</t>
+  </si>
+  <si>
+    <t>Chata</t>
+  </si>
+  <si>
+    <t>Samba</t>
+  </si>
+  <si>
+    <t>Reggue</t>
+  </si>
+  <si>
+    <t>Yo</t>
+  </si>
+  <si>
+    <t>Angeles Azules</t>
+  </si>
+  <si>
+    <t>Negrito de ojos claros</t>
+  </si>
+  <si>
+    <t>Bob Esponja</t>
+  </si>
+  <si>
+    <t>A bailar prros</t>
+  </si>
+  <si>
+    <t>A bailasx2</t>
+  </si>
+  <si>
+    <t>La modelo</t>
+  </si>
+  <si>
+    <t>F es la familia</t>
+  </si>
+  <si>
+    <t>Caballito Nicoyano</t>
+  </si>
+  <si>
+    <t>El porcio</t>
+  </si>
+  <si>
+    <t>BaBunny</t>
+  </si>
+  <si>
+    <t>Soi Pior</t>
+  </si>
+  <si>
+    <t>Soi mas Pior</t>
+  </si>
+  <si>
+    <t>Brasileño</t>
+  </si>
+  <si>
+    <t>Roberto Marley</t>
+  </si>
+  <si>
+    <t>Krippy Kush</t>
+  </si>
+  <si>
+    <t>Mota y mas Mota</t>
+  </si>
+  <si>
+    <t>Neymar es gei</t>
+  </si>
+  <si>
+    <t>Farru</t>
+  </si>
+  <si>
+    <t>Album4</t>
+  </si>
+  <si>
+    <t>Album5</t>
+  </si>
+  <si>
+    <t>Album6</t>
+  </si>
+  <si>
+    <t>Album7</t>
+  </si>
+  <si>
+    <t>Album8</t>
+  </si>
+  <si>
+    <t>Album9</t>
+  </si>
+  <si>
+    <t>Album10</t>
   </si>
 </sst>
 </file>
@@ -133,7 +229,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -429,32 +525,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E251E6-7C9C-449E-BDAA-2BE03F22322D}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D1">
         <v>5.0999999999999996</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -462,19 +562,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>5.2</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -482,19 +582,159 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>5.3</v>
       </c>
       <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>2.1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>3.4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>7.2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>2.23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>5.2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>